<commit_message>
Updated pokemon csv, fixed text allignment for move text in BattleBar
</commit_message>
<xml_diff>
--- a/PokemonBattleGame/Resources/Pokemon_List.xlsx
+++ b/PokemonBattleGame/Resources/Pokemon_List.xlsx
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F39" workbookViewId="0">
-      <selection activeCell="T56" sqref="T56"/>
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,7 +1475,7 @@
         <v>157</v>
       </c>
       <c r="Q6">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="R6">
         <v>17</v>
@@ -1484,7 +1484,7 @@
         <v>18</v>
       </c>
       <c r="T6">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -2281,13 +2281,13 @@
         <v>150</v>
       </c>
       <c r="Q19">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="R19">
         <v>18</v>
       </c>
       <c r="S19">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="T19">
         <v>3</v>
@@ -2405,7 +2405,7 @@
         <v>156</v>
       </c>
       <c r="Q21">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="R21">
         <v>17</v>
@@ -2414,7 +2414,7 @@
         <v>18</v>
       </c>
       <c r="T21">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:20">

</xml_diff>